<commit_message>
BigData HW2. Final step. Ready for assessment.
</commit_message>
<xml_diff>
--- a/bigdata/hw2.hdfs/performance report.xlsx
+++ b/bigdata/hw2.hdfs/performance report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>process time</t>
   </si>
@@ -32,22 +32,208 @@
     <t>memory</t>
   </si>
   <si>
-    <t>default options (x64 JVM)</t>
-  </si>
-  <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>319s</t>
+  </si>
+  <si>
+    <t>cpu max load</t>
+  </si>
+  <si>
+    <t>80,9%</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>3,3G</t>
+  </si>
+  <si>
+    <t>GC max activity</t>
+  </si>
+  <si>
+    <t>23,2%</t>
+  </si>
+  <si>
+    <t>casses loaded</t>
+  </si>
+  <si>
+    <t>default parameters</t>
+  </si>
+  <si>
+    <t>295s</t>
+  </si>
+  <si>
+    <t>41,9%</t>
+  </si>
+  <si>
+    <t>7,2%</t>
+  </si>
+  <si>
+    <t>8G</t>
+  </si>
+  <si>
+    <t>4,5G</t>
+  </si>
+  <si>
+    <t>heap max</t>
+  </si>
+  <si>
+    <t>max heap used</t>
+  </si>
+  <si>
+    <t>metaspace max</t>
+  </si>
+  <si>
+    <t>max metaspace used</t>
+  </si>
+  <si>
+    <t>1G</t>
+  </si>
+  <si>
+    <t>20M</t>
+  </si>
+  <si>
+    <t>300s</t>
+  </si>
+  <si>
+    <t>4,6G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Xms8g -Xmx8g -Xnoclassgc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Xms8g -Xmx8g</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -XX:+AggressiveOpts</t>
+  </si>
+  <si>
+    <t>293s</t>
+  </si>
+  <si>
+    <t>532s</t>
+  </si>
+  <si>
+    <t>17G</t>
+  </si>
+  <si>
+    <t>3,6G</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -XX:+UseG1GC</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -Xmn2g -XX:+UseG1GC -XX:-OmitStackTraceInFastThrow -XX:SurvivorRatio=2 -XX:NewSize=4g -XX:MaxNewSize=5g -XX:+UseStringDeduplication</t>
+  </si>
+  <si>
+    <t>866s</t>
+  </si>
+  <si>
+    <t>5,6G</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -XX:+UseSerialGC</t>
+  </si>
+  <si>
+    <t>314s</t>
+  </si>
+  <si>
+    <t>3G</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -XX:+UseConcMarkSweepGC</t>
+  </si>
+  <si>
+    <t>310s</t>
+  </si>
+  <si>
+    <t>2,2G</t>
+  </si>
+  <si>
+    <t>-Xms4g -Xmx8g -XX:+UseParallelGC</t>
+  </si>
+  <si>
+    <t>287s</t>
+  </si>
+  <si>
+    <t>321s</t>
+  </si>
+  <si>
+    <t>53,8%</t>
+  </si>
+  <si>
+    <t>12,3%</t>
+  </si>
+  <si>
+    <t>-Xms8g -Xmx8g -XX:+UseParallelGC -XX:ConcGCThreads=5 -XX:ParallelGCThreads=5</t>
+  </si>
+  <si>
+    <t>38,7%</t>
+  </si>
+  <si>
+    <t>16,8%</t>
+  </si>
+  <si>
+    <t>4,2G</t>
+  </si>
+  <si>
+    <t>-Xms8g -Xmx8g -XX:+UseSerialGC</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -71,8 +257,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,37 +560,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3563</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3566</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3565</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3531</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3565</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3565</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3526</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3566</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3537</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3566</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3565</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>